<commit_message>
Add ProductDetailsPage.java Add test for selecting item, selecting its property based on data from excel and add it to the card
</commit_message>
<xml_diff>
--- a/inits/Credentials.xlsx
+++ b/inits/Credentials.xlsx
@@ -567,10 +567,10 @@
         <v>SanityTest</v>
       </c>
       <c r="B6" t="str">
-        <v>testnew1@abv.bg</v>
+        <v>test123@abv.bg</v>
       </c>
       <c r="C6" t="str">
-        <v>alabala</v>
+        <v>123456</v>
       </c>
       <c r="D6" t="str">
         <v>CHROME</v>
@@ -579,7 +579,7 @@
         <v>http://www.automationpractice.pl/index.php?</v>
       </c>
       <c r="F6" t="str">
-        <v>Ivan Ivanov</v>
+        <v>Test Testing</v>
       </c>
       <c r="G6" t="str">
         <v/>
@@ -599,7 +599,7 @@
         <v>RegistrationDDT</v>
       </c>
       <c r="B7" t="str">
-        <v>testnew5@abv.bg</v>
+        <v>testnew1@abv.bg</v>
       </c>
       <c r="C7" t="str">
         <v>alabala</v>

</xml_diff>